<commit_message>
cleaned up a bunch of stuff
</commit_message>
<xml_diff>
--- a/Design/Configure/AddModulesConfig.xlsx
+++ b/Design/Configure/AddModulesConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyash\Documents\UiPath\LazyFramework\Configure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyash\Documents\UiPath\LazyFramework\Design\Configure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B662463-7EB7-4CB0-97DF-9792AD25BAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB4CF4-A019-4507-8C06-C0CBEBE6D6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27360" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="36780" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelFiles" sheetId="5" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t>ModuleConfig</t>
   </si>
   <si>
-    <t>Configure\Modules.xlsx</t>
-  </si>
-  <si>
     <t>The path to the configuration file for modules.</t>
+  </si>
+  <si>
+    <t>Design\Configure\Modules.xlsx</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,10 +407,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>